<commit_message>
TODO - Answer todo question
</commit_message>
<xml_diff>
--- a/guidance.xlsx
+++ b/guidance.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studenthcmusedu-my.sharepoint.com/personal/18120201_student_hcmus_edu_vn/Documents/BS/Term 6/Phân tích dữ liệu thông minh/Bài tập/Đồ án thực hành/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studenthcmusedu-my.sharepoint.com/personal/20280083_student_hcmus_edu_vn/Documents/Jupyter Hub/KHDL-PythonForDS/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{AB5F8B96-2BE1-3841-806F-9C760EEAAB5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DF0FBDE5-604C-5F40-861E-9C87161B8AF8}"/>
   <bookViews>
-    <workbookView xWindow="920" yWindow="500" windowWidth="24680" windowHeight="14620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="accidentsguidance" sheetId="1" r:id="rId1"/>
@@ -831,9 +831,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
@@ -1201,22 +1200,22 @@
   <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="49" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.796875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="34" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.69921875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.69921875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="49" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="G1" t="s">
         <v>74</v>
       </c>
@@ -1224,468 +1223,468 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="6">
+    <row r="3" spans="1:11" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="5">
         <v>1</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="9">
         <v>1</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3" s="5">
         <v>1</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" t="s">
         <v>26</v>
       </c>
-      <c r="J3" s="6">
+      <c r="J3" s="5">
         <v>1</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="K3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="6">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="5">
         <v>2</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <v>2</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="5">
         <v>2</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" t="s">
         <v>27</v>
       </c>
-      <c r="J4" s="6">
+      <c r="J4" s="5">
         <v>2</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="K4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="6">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="5">
         <v>3</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="5">
         <v>3</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="5">
         <v>3</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H5" t="s">
         <v>28</v>
       </c>
-      <c r="J5" s="6">
+      <c r="J5" s="5">
         <v>3</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="K5" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="6">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="5">
         <v>4</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="5">
         <v>4</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="5">
         <v>4</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" t="s">
         <v>29</v>
       </c>
-      <c r="J6" s="6">
+      <c r="J6" s="5">
         <v>4</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="K6" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="6">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="5">
         <v>5</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="5">
         <v>5</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" t="s">
         <v>21</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="5">
         <v>5</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" t="s">
         <v>30</v>
       </c>
-      <c r="J7" s="6">
+      <c r="J7" s="5">
         <v>5</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="K7" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="8">
+    <row r="8" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="7">
         <v>6</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="5">
         <v>6</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" t="s">
         <v>22</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="5">
         <v>6</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H8" t="s">
         <v>31</v>
       </c>
-      <c r="J8" s="6">
+      <c r="J8" s="5">
         <v>6</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="K8" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D9" s="8">
+    <row r="9" spans="1:11" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D9" s="7">
         <v>7</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="5">
         <v>7</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="H9" t="s">
         <v>32</v>
       </c>
-      <c r="J9" s="6">
+      <c r="J9" s="5">
         <v>7</v>
       </c>
-      <c r="K9" s="1" t="s">
+      <c r="K9" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+    <row r="10" spans="1:11" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G10" s="6">
+      <c r="G10" s="5">
         <v>8</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="H10" t="s">
         <v>33</v>
       </c>
-      <c r="J10" s="6">
+      <c r="J10" s="5">
         <v>8</v>
       </c>
-      <c r="K10" s="1" t="s">
+      <c r="K10" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="6">
+    <row r="11" spans="1:11" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="5">
         <v>1</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="8">
+      <c r="G11" s="7">
         <v>9</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="H11" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="J11" s="6">
+      <c r="J11" s="5">
         <v>9</v>
       </c>
-      <c r="K11" s="1" t="s">
+      <c r="K11" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="6">
+    <row r="12" spans="1:11" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="5">
         <v>2</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="J12" s="6">
+      <c r="J12" s="5">
         <v>10</v>
       </c>
-      <c r="K12" s="1" t="s">
+      <c r="K12" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="6">
+    <row r="13" spans="1:11" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="5">
         <v>3</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J13" s="6">
+      <c r="J13" s="5">
         <v>11</v>
       </c>
-      <c r="K13" s="1" t="s">
+      <c r="K13" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="6">
+    <row r="14" spans="1:11" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="5">
         <v>4</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="J14" s="6">
+      <c r="J14" s="5">
         <v>12</v>
       </c>
-      <c r="K14" s="1" t="s">
+      <c r="K14" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="8">
+    <row r="15" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="7">
         <v>5</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="J15" s="6">
+      <c r="J15" s="5">
         <v>13</v>
       </c>
-      <c r="K15" s="1" t="s">
+      <c r="K15" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="D16" t="s">
         <v>75</v>
       </c>
-      <c r="J16" s="6">
+      <c r="J16" s="5">
         <v>14</v>
       </c>
-      <c r="K16" s="1" t="s">
+      <c r="K16" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
+    <row r="17" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E17" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="G17" s="4" t="s">
+      <c r="G17" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="H17" s="3" t="s">
+      <c r="H17" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="J17" s="6">
+      <c r="J17" s="5">
         <v>15</v>
       </c>
-      <c r="K17" s="1" t="s">
+      <c r="K17" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="6">
+    <row r="18" spans="1:11" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="5">
         <v>1</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D18" s="6">
+      <c r="D18" s="5">
         <v>1</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E18" t="s">
         <v>42</v>
       </c>
-      <c r="G18" s="6">
+      <c r="G18" s="5">
         <v>1</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="H18" t="s">
         <v>47</v>
       </c>
-      <c r="J18" s="6">
+      <c r="J18" s="5">
         <v>16</v>
       </c>
-      <c r="K18" s="1" t="s">
+      <c r="K18" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="6">
+    <row r="19" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="5">
         <v>2</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D19" s="6">
+      <c r="D19" s="5">
         <v>2</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E19" t="s">
         <v>43</v>
       </c>
-      <c r="G19" s="8">
+      <c r="G19" s="7">
         <v>2</v>
       </c>
-      <c r="H19" s="2" t="s">
+      <c r="H19" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="J19" s="6">
+      <c r="J19" s="5">
         <v>17</v>
       </c>
-      <c r="K19" s="1" t="s">
+      <c r="K19" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="8">
+    <row r="20" spans="1:11" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="7">
         <v>3</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D20" s="8">
+      <c r="D20" s="7">
         <v>3</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="E20" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="J20" s="6">
+      <c r="J20" s="5">
         <v>18</v>
       </c>
-      <c r="K20" s="1" t="s">
+      <c r="K20" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="J21" s="6">
+    <row r="21" spans="1:11" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="J21" s="5">
         <v>19</v>
       </c>
-      <c r="K21" s="1" t="s">
+      <c r="K21" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="J22" s="6">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J22" s="5">
         <v>20</v>
       </c>
-      <c r="K22" s="1" t="s">
+      <c r="K22" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="J23" s="6">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J23" s="5">
         <v>21</v>
       </c>
-      <c r="K23" s="1" t="s">
+      <c r="K23" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="J24" s="6">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J24" s="5">
         <v>22</v>
       </c>
-      <c r="K24" s="1" t="s">
+      <c r="K24" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="J25" s="6">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J25" s="5">
         <v>90</v>
       </c>
-      <c r="K25" s="1" t="s">
+      <c r="K25" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J26" s="8">
+    <row r="26" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J26" s="7">
         <v>97</v>
       </c>
-      <c r="K26" s="2" t="s">
+      <c r="K26" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:11" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>